<commit_message>
weekly commit before data removal
</commit_message>
<xml_diff>
--- a/data_output/weekly_report_output.xlsx
+++ b/data_output/weekly_report_output.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">CDC-061</t>
   </si>
   <si>
-    <t xml:space="preserve">BERTHOUD RESERVIOR</t>
+    <t xml:space="preserve">BERTHOUD RESERVOIR</t>
   </si>
   <si>
     <t xml:space="preserve">CDC-062</t>
@@ -728,18 +728,27 @@
     <t xml:space="preserve">abund_Tarsalis</t>
   </si>
   <si>
+    <t xml:space="preserve">abund_All</t>
+  </si>
+  <si>
     <t xml:space="preserve">pir_Pipiens</t>
   </si>
   <si>
     <t xml:space="preserve">pir_Tarsalis</t>
   </si>
   <si>
+    <t xml:space="preserve">pir_All</t>
+  </si>
+  <si>
     <t xml:space="preserve">vi_Pipiens</t>
   </si>
   <si>
     <t xml:space="preserve">vi_Tarsalis</t>
   </si>
   <si>
+    <t xml:space="preserve">vi_All</t>
+  </si>
+  <si>
     <t xml:space="preserve">all_vi</t>
   </si>
   <si>
@@ -800,6 +809,9 @@
     <t xml:space="preserve">collected_Tarsalis</t>
   </si>
   <si>
+    <t xml:space="preserve">collected_All</t>
+  </si>
+  <si>
     <t xml:space="preserve">all_collected</t>
   </si>
   <si>
@@ -863,6 +875,9 @@
     <t xml:space="preserve">examined_Tarsalis</t>
   </si>
   <si>
+    <t xml:space="preserve">examined_All</t>
+  </si>
+  <si>
     <t xml:space="preserve">all_examined</t>
   </si>
   <si>
@@ -872,6 +887,9 @@
     <t xml:space="preserve">pool_Tarsalis</t>
   </si>
   <si>
+    <t xml:space="preserve">pool_All</t>
+  </si>
+  <si>
     <t xml:space="preserve">all_pool</t>
   </si>
   <si>
@@ -879,6 +897,9 @@
   </si>
   <si>
     <t xml:space="preserve">pos_pool_Tarsalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_pool_All</t>
   </si>
   <si>
     <t xml:space="preserve">all_pos_pool</t>
@@ -8051,6 +8072,15 @@
       <c r="H1" t="s">
         <v>240</v>
       </c>
+      <c r="I1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -8063,7 +8093,7 @@
         <v>9.78</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>18.56</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -8075,6 +8105,15 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8089,7 +8128,7 @@
         <v>14.5</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -8101,6 +8140,15 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8115,7 +8163,7 @@
         <v>20.33</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>25.8</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -8127,6 +8175,15 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8141,7 +8198,7 @@
         <v>9.25</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -8153,6 +8210,15 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8167,7 +8233,7 @@
         <v>14.57</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>20.45</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -8179,6 +8245,15 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8193,7 +8268,7 @@
         <v>47.17</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -8205,6 +8280,15 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8219,18 +8303,27 @@
         <v>59.11</v>
       </c>
       <c r="D8" t="n">
+        <v>64.55</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.0179</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
       <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.00150890782339272</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.0974</v>
       </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0974</v>
+      </c>
+      <c r="K8" t="n">
         <v>0.0974</v>
       </c>
     </row>
@@ -8242,10 +8335,10 @@
       <c r="C9" t="n">
         <v>45</v>
       </c>
-      <c r="D9"/>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
+      <c r="D9" t="n">
+        <v>45</v>
+      </c>
+      <c r="E9"/>
       <c r="F9" t="n">
         <v>0</v>
       </c>
@@ -8253,6 +8346,15 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8272,55 +8374,55 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="J1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="L1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="M1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="N1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="P1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Q1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2">
@@ -8494,7 +8596,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0121</v>
+        <v>0.0108833333333333</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -8506,7 +8608,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0042</v>
+        <v>0.00495</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -8547,7 +8649,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0556</v>
+        <v>0.0472833333333333</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -8559,19 +8661,19 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.02</v>
+        <v>0.0148333333333333</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0654</v>
+        <v>0.0538833333333333</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0433</v>
+        <v>0.0699833333333333</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
@@ -8588,49 +8690,49 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0186</v>
+        <v>0.0148166666666667</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0198</v>
+        <v>0.0159166666666667</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1972</v>
+        <v>0.168533333333333</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0876</v>
+        <v>0.0483</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0978</v>
+        <v>0.0791</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0359</v>
+        <v>0.0269</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1098</v>
+        <v>0.0974</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>0.111833333333333</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.1351</v>
+        <v>0.138333333333333</v>
       </c>
     </row>
     <row r="8">
@@ -8639,35 +8741,35 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="n">
-        <v>0.1592</v>
+        <v>0.0900666666666667</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="n">
-        <v>0.2522</v>
+        <v>0.209233333333333</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.2559</v>
+        <v>0.209516666666667</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="n">
-        <v>0.1465</v>
+        <v>0.153133333333333</v>
       </c>
       <c r="J8"/>
       <c r="K8" t="n">
-        <v>0.2067</v>
+        <v>0.175416666666667</v>
       </c>
       <c r="L8"/>
       <c r="M8" t="n">
-        <v>0.1323</v>
+        <v>0.142783333333333</v>
       </c>
       <c r="N8"/>
       <c r="O8" t="n">
-        <v>0.0463</v>
+        <v>0.1026</v>
       </c>
       <c r="P8"/>
       <c r="Q8" t="n">
-        <v>0.2173</v>
+        <v>0.2489</v>
       </c>
     </row>
     <row r="9">
@@ -8676,35 +8778,35 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="n">
-        <v>0.0577</v>
+        <v>0.06815</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="n">
-        <v>0.1871</v>
+        <v>0.164333333333333</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.2048</v>
+        <v>0.168366666666667</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="n">
-        <v>0.1597</v>
+        <v>0.163933333333333</v>
       </c>
       <c r="J9"/>
       <c r="K9" t="n">
-        <v>0.1591</v>
+        <v>0.14645</v>
       </c>
       <c r="L9"/>
       <c r="M9" t="n">
-        <v>0.5115</v>
+        <v>0.510433333333333</v>
       </c>
       <c r="N9"/>
       <c r="O9" t="n">
-        <v>0.0911</v>
+        <v>0.175916666666667</v>
       </c>
       <c r="P9"/>
       <c r="Q9" t="n">
-        <v>0.0647</v>
+        <v>0.0634666666666667</v>
       </c>
     </row>
     <row r="10">
@@ -8713,35 +8815,35 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="n">
-        <v>0.1396</v>
+        <v>0.11595</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="n">
-        <v>0.089</v>
+        <v>0.0856333333333333</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.4422</v>
+        <v>0.407366666666667</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="n">
-        <v>0.1263</v>
+        <v>0.110583333333333</v>
       </c>
       <c r="J10"/>
       <c r="K10" t="n">
-        <v>0.2357</v>
+        <v>0.226333333333333</v>
       </c>
       <c r="L10"/>
       <c r="M10" t="n">
-        <v>0.3126</v>
+        <v>0.264016666666667</v>
       </c>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>0.0681</v>
+        <v>0.140983333333333</v>
       </c>
       <c r="P10"/>
       <c r="Q10" t="n">
-        <v>0.0687</v>
+        <v>0.0679333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -8750,35 +8852,35 @@
       </c>
       <c r="B11"/>
       <c r="C11" t="n">
-        <v>0.1792</v>
+        <v>0.199833333333333</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="n">
-        <v>0.2229</v>
+        <v>0.18375</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.2439</v>
+        <v>0.242816666666667</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="n">
-        <v>0.2371</v>
+        <v>0.200366666666667</v>
       </c>
       <c r="J11"/>
       <c r="K11" t="n">
-        <v>0.2312</v>
+        <v>0.218516666666667</v>
       </c>
       <c r="L11"/>
       <c r="M11" t="n">
-        <v>0.3653</v>
+        <v>0.345516666666667</v>
       </c>
       <c r="N11"/>
       <c r="O11" t="n">
-        <v>0.2797</v>
+        <v>0.5082</v>
       </c>
       <c r="P11"/>
       <c r="Q11" t="n">
-        <v>0.1411</v>
+        <v>0.1336</v>
       </c>
     </row>
     <row r="12">
@@ -8787,35 +8889,35 @@
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>0.1574</v>
+        <v>0.13545</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="n">
-        <v>0.4383</v>
+        <v>0.497183333333333</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.2533</v>
+        <v>0.226766666666667</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="n">
-        <v>0.23</v>
+        <v>0.225083333333333</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="n">
-        <v>0.2705</v>
+        <v>0.272666666666667</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="n">
-        <v>0.3722</v>
+        <v>0.3657</v>
       </c>
       <c r="N12"/>
       <c r="O12" t="n">
-        <v>0.0221</v>
+        <v>0.0362166666666667</v>
       </c>
       <c r="P12"/>
       <c r="Q12" t="n">
-        <v>0.0666</v>
+        <v>0.0620666666666667</v>
       </c>
     </row>
     <row r="13">
@@ -8824,35 +8926,35 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="n">
-        <v>0.1761</v>
+        <v>0.155316666666667</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="n">
-        <v>0.346</v>
+        <v>0.338366666666667</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.329</v>
+        <v>0.271366666666667</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="n">
-        <v>0.2903</v>
+        <v>0.23865</v>
       </c>
       <c r="J13"/>
       <c r="K13" t="n">
-        <v>0.2955</v>
+        <v>0.259483333333333</v>
       </c>
       <c r="L13"/>
       <c r="M13" t="n">
-        <v>0.244</v>
+        <v>0.201133333333333</v>
       </c>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>0.0974</v>
+        <v>0.2655</v>
       </c>
       <c r="P13"/>
       <c r="Q13" t="n">
-        <v>0.0683</v>
+        <v>0.0643</v>
       </c>
     </row>
     <row r="14">
@@ -8861,31 +8963,31 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="n">
-        <v>0.0967</v>
+        <v>0.08825</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="n">
-        <v>0.2794</v>
+        <v>0.319216666666667</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.302</v>
+        <v>0.325816666666667</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="n">
-        <v>0.1184</v>
+        <v>0.0765</v>
       </c>
       <c r="J14"/>
       <c r="K14" t="n">
-        <v>0.2162</v>
+        <v>0.229533333333333</v>
       </c>
       <c r="L14"/>
       <c r="M14" t="n">
-        <v>0.3002</v>
+        <v>0.258666666666667</v>
       </c>
       <c r="N14"/>
       <c r="O14" t="n">
-        <v>0.0683</v>
+        <v>0.0956333333333333</v>
       </c>
       <c r="P14"/>
       <c r="Q14" t="n">
@@ -8898,27 +9000,27 @@
       </c>
       <c r="B15"/>
       <c r="C15" t="n">
-        <v>0.0542</v>
+        <v>0.0301</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="n">
-        <v>0.0847</v>
+        <v>0.0892833333333333</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.0838</v>
+        <v>0.0606666666666667</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="n">
-        <v>0.0314</v>
+        <v>0.0352</v>
       </c>
       <c r="J15"/>
       <c r="K15" t="n">
-        <v>0.07</v>
+        <v>0.0651333333333333</v>
       </c>
       <c r="L15"/>
       <c r="M15" t="n">
-        <v>0.1316</v>
+        <v>0.1397</v>
       </c>
       <c r="N15"/>
       <c r="O15"/>
@@ -8933,15 +9035,15 @@
       </c>
       <c r="B16"/>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.013675</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="n">
-        <v>0.1885</v>
+        <v>0.1714</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.0379</v>
+        <v>0.0285</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="n">
@@ -8949,7 +9051,7 @@
       </c>
       <c r="J16"/>
       <c r="K16" t="n">
-        <v>0.0546</v>
+        <v>0.054475</v>
       </c>
       <c r="L16"/>
       <c r="M16"/>
@@ -8979,25 +9081,31 @@
         <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G1" t="s">
         <v>234</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>235</v>
       </c>
-      <c r="H1" t="s">
-        <v>262</v>
+      <c r="I1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="2">
@@ -9014,15 +9122,21 @@
         <v>167</v>
       </c>
       <c r="E2" t="n">
+        <v>167</v>
+      </c>
+      <c r="F2" t="n">
         <v>9</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>8.78</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>9.78</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
+        <v>18.56</v>
+      </c>
+      <c r="J2" t="n">
         <v>18.56</v>
       </c>
     </row>
@@ -9040,15 +9154,21 @@
         <v>205</v>
       </c>
       <c r="E3" t="n">
+        <v>205</v>
+      </c>
+      <c r="F3" t="n">
         <v>10</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>6</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>14.5</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="J3" t="n">
         <v>20.5</v>
       </c>
     </row>
@@ -9066,15 +9186,21 @@
         <v>387</v>
       </c>
       <c r="E4" t="n">
+        <v>387</v>
+      </c>
+      <c r="F4" t="n">
         <v>15</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>5.47</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>20.33</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="J4" t="n">
         <v>25.8</v>
       </c>
     </row>
@@ -9092,15 +9218,21 @@
         <v>100</v>
       </c>
       <c r="E5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" t="n">
         <v>8</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>3.25</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>9.25</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="J5" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -9118,15 +9250,21 @@
         <v>859</v>
       </c>
       <c r="E6" t="n">
+        <v>859</v>
+      </c>
+      <c r="F6" t="n">
         <v>42</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>5.88</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>14.57</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
+        <v>20.45</v>
+      </c>
+      <c r="J6" t="n">
         <v>20.45</v>
       </c>
     </row>
@@ -9144,15 +9282,21 @@
         <v>306</v>
       </c>
       <c r="E7" t="n">
+        <v>306</v>
+      </c>
+      <c r="F7" t="n">
         <v>6</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>3.83</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>47.17</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
+        <v>51</v>
+      </c>
+      <c r="J7" t="n">
         <v>51</v>
       </c>
     </row>
@@ -9170,15 +9314,21 @@
         <v>581</v>
       </c>
       <c r="E8" t="n">
+        <v>581</v>
+      </c>
+      <c r="F8" t="n">
         <v>9</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>5.44</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>59.11</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
+        <v>64.55</v>
+      </c>
+      <c r="J8" t="n">
         <v>64.55</v>
       </c>
     </row>
@@ -9196,13 +9346,19 @@
         <v>225</v>
       </c>
       <c r="E9" t="n">
+        <v>225</v>
+      </c>
+      <c r="F9" t="n">
         <v>5</v>
       </c>
-      <c r="F9"/>
-      <c r="G9" t="n">
+      <c r="G9"/>
+      <c r="H9" t="n">
         <v>45</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
+        <v>45</v>
+      </c>
+      <c r="J9" t="n">
         <v>45</v>
       </c>
     </row>
@@ -9222,55 +9378,55 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="I1" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="J1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="K1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="L1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="M1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="O1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2">
@@ -9278,7 +9434,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="n">
-        <v>1.67</v>
+        <v>1.66</v>
       </c>
       <c r="C2" t="n">
         <v>3.78</v>
@@ -9290,19 +9446,19 @@
         <v>3.45</v>
       </c>
       <c r="F2" t="n">
-        <v>1.67</v>
+        <v>1.78</v>
       </c>
       <c r="G2" t="n">
-        <v>5.73</v>
+        <v>5.735</v>
       </c>
       <c r="H2" t="n">
-        <v>2.67</v>
+        <v>2.66</v>
       </c>
       <c r="I2" t="n">
         <v>4.89</v>
       </c>
       <c r="J2" t="n">
-        <v>2.19</v>
+        <v>2.24</v>
       </c>
       <c r="K2" t="n">
         <v>4.62</v>
@@ -9314,10 +9470,10 @@
         <v>18.22</v>
       </c>
       <c r="N2" t="n">
-        <v>0.67</v>
+        <v>0.6</v>
       </c>
       <c r="O2" t="n">
-        <v>6.15</v>
+        <v>12.2</v>
       </c>
       <c r="P2"/>
       <c r="Q2"/>
@@ -9330,47 +9486,47 @@
         <v>1.67</v>
       </c>
       <c r="C3" t="n">
-        <v>4.96</v>
+        <v>6.3325</v>
       </c>
       <c r="D3" t="n">
         <v>1.9</v>
       </c>
       <c r="E3" t="n">
-        <v>4.68</v>
+        <v>5.04</v>
       </c>
       <c r="F3" t="n">
         <v>2.2</v>
       </c>
       <c r="G3" t="n">
-        <v>4.12</v>
+        <v>6.346</v>
       </c>
       <c r="H3" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="I3" t="n">
-        <v>2.89</v>
+        <v>3.044</v>
       </c>
       <c r="J3" t="n">
         <v>1.84</v>
       </c>
       <c r="K3" t="n">
-        <v>4.17</v>
+        <v>5.084</v>
       </c>
       <c r="L3" t="n">
-        <v>5.33</v>
+        <v>5.34</v>
       </c>
       <c r="M3" t="n">
-        <v>20.23</v>
+        <v>20.2233333333333</v>
       </c>
       <c r="N3" t="n">
-        <v>8.44</v>
+        <v>7.6</v>
       </c>
       <c r="O3" t="n">
-        <v>7.6</v>
+        <v>15.5416666666667</v>
       </c>
       <c r="P3"/>
       <c r="Q3" t="n">
-        <v>15.4</v>
+        <v>15.725</v>
       </c>
     </row>
     <row r="4">
@@ -9378,50 +9534,50 @@
         <v>25</v>
       </c>
       <c r="B4" t="n">
-        <v>5.89</v>
+        <v>6.63</v>
       </c>
       <c r="C4" t="n">
-        <v>6.13</v>
+        <v>5.61</v>
       </c>
       <c r="D4" t="n">
-        <v>13.4</v>
+        <v>14.89</v>
       </c>
       <c r="E4" t="n">
-        <v>10.5</v>
+        <v>9.26666666666667</v>
       </c>
       <c r="F4" t="n">
         <v>6.47</v>
       </c>
       <c r="G4" t="n">
-        <v>16.52</v>
+        <v>16.9683333333333</v>
       </c>
       <c r="H4" t="n">
-        <v>1.67</v>
+        <v>1.66</v>
       </c>
       <c r="I4" t="n">
-        <v>3.73</v>
+        <v>3.64833333333333</v>
       </c>
       <c r="J4" t="n">
-        <v>6.95</v>
+        <v>7.3</v>
       </c>
       <c r="K4" t="n">
-        <v>10.27</v>
+        <v>10.0083333333333</v>
       </c>
       <c r="L4" t="n">
-        <v>16.67</v>
+        <v>16.66</v>
       </c>
       <c r="M4" t="n">
-        <v>41.43</v>
+        <v>37.6666666666667</v>
       </c>
       <c r="N4" t="n">
-        <v>18.89</v>
+        <v>17</v>
       </c>
       <c r="O4" t="n">
-        <v>15.07</v>
+        <v>25.375</v>
       </c>
       <c r="P4"/>
       <c r="Q4" t="n">
-        <v>18.67</v>
+        <v>18.5033333333333</v>
       </c>
     </row>
     <row r="5">
@@ -9429,52 +9585,52 @@
         <v>26</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>34.38</v>
+        <v>32.3683333333333</v>
       </c>
       <c r="D5" t="n">
         <v>29</v>
       </c>
       <c r="E5" t="n">
-        <v>38.48</v>
+        <v>35.0166666666667</v>
       </c>
       <c r="F5" t="n">
         <v>15.6</v>
       </c>
       <c r="G5" t="n">
-        <v>60.44</v>
+        <v>56.7516666666667</v>
       </c>
       <c r="H5" t="n">
         <v>2.56</v>
       </c>
       <c r="I5" t="n">
-        <v>22.78</v>
+        <v>23.63</v>
       </c>
       <c r="J5" t="n">
-        <v>14.4</v>
+        <v>14.74</v>
       </c>
       <c r="K5" t="n">
-        <v>42</v>
+        <v>39.6616666666667</v>
       </c>
       <c r="L5" t="n">
         <v>34.33</v>
       </c>
       <c r="M5" t="n">
-        <v>111.07</v>
+        <v>96.9983333333333</v>
       </c>
       <c r="N5" t="n">
-        <v>57.67</v>
+        <v>51.9</v>
       </c>
       <c r="O5" t="n">
-        <v>20.24</v>
+        <v>44.4666666666667</v>
       </c>
       <c r="P5" t="n">
         <v>20</v>
       </c>
       <c r="Q5" t="n">
-        <v>22.2</v>
+        <v>21.73</v>
       </c>
     </row>
     <row r="6">
@@ -9482,52 +9638,52 @@
         <v>27</v>
       </c>
       <c r="B6" t="n">
-        <v>6.78</v>
+        <v>6.77</v>
       </c>
       <c r="C6" t="n">
-        <v>25.33</v>
+        <v>27.89</v>
       </c>
       <c r="D6" t="n">
         <v>20.3</v>
       </c>
       <c r="E6" t="n">
-        <v>81.84</v>
+        <v>80.7</v>
       </c>
       <c r="F6" t="n">
         <v>9.87</v>
       </c>
       <c r="G6" t="n">
-        <v>111.17</v>
+        <v>103.38</v>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>16.76</v>
+        <v>18.1633333333333</v>
       </c>
       <c r="J6" t="n">
         <v>10</v>
       </c>
       <c r="K6" t="n">
-        <v>66.62</v>
+        <v>64.4683333333333</v>
       </c>
       <c r="L6" t="n">
         <v>31.67</v>
       </c>
       <c r="M6" t="n">
-        <v>217.9</v>
+        <v>190.471666666667</v>
       </c>
       <c r="N6" t="n">
-        <v>62.78</v>
+        <v>56.5</v>
       </c>
       <c r="O6" t="n">
-        <v>30.96</v>
+        <v>74.1083333333333</v>
       </c>
       <c r="P6" t="n">
         <v>24.6</v>
       </c>
       <c r="Q6" t="n">
-        <v>45.8</v>
+        <v>45.2733333333333</v>
       </c>
     </row>
     <row r="7">
@@ -9538,49 +9694,49 @@
         <v>18.56</v>
       </c>
       <c r="C7" t="n">
-        <v>61.87</v>
+        <v>59.7966666666667</v>
       </c>
       <c r="D7" t="n">
         <v>20.5</v>
       </c>
       <c r="E7" t="n">
-        <v>99.18</v>
+        <v>97.7333333333333</v>
       </c>
       <c r="F7" t="n">
         <v>25.8</v>
       </c>
       <c r="G7" t="n">
-        <v>164.35</v>
+        <v>150.365</v>
       </c>
       <c r="H7" t="n">
-        <v>11.11</v>
+        <v>12.5</v>
       </c>
       <c r="I7" t="n">
-        <v>72.98</v>
+        <v>65.15</v>
       </c>
       <c r="J7" t="n">
-        <v>19.98</v>
+        <v>20.45</v>
       </c>
       <c r="K7" t="n">
-        <v>108.62</v>
+        <v>101.335</v>
       </c>
       <c r="L7" t="n">
         <v>51</v>
       </c>
       <c r="M7" t="n">
-        <v>179.43</v>
+        <v>170.47</v>
       </c>
       <c r="N7" t="n">
-        <v>64.56</v>
+        <v>64.55</v>
       </c>
       <c r="O7" t="n">
-        <v>39.67</v>
+        <v>109.425</v>
       </c>
       <c r="P7" t="n">
         <v>45</v>
       </c>
       <c r="Q7" t="n">
-        <v>39.73</v>
+        <v>39.3233333333333</v>
       </c>
     </row>
     <row r="8">
@@ -9589,35 +9745,35 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="n">
-        <v>83.78</v>
+        <v>76.4066666666667</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="n">
-        <v>180.12</v>
+        <v>153.333333333333</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>159.96</v>
+        <v>140.753333333333</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="n">
-        <v>66.58</v>
+        <v>59.6116666666667</v>
       </c>
       <c r="J8"/>
       <c r="K8" t="n">
-        <v>129.16</v>
+        <v>113.23</v>
       </c>
       <c r="L8"/>
       <c r="M8" t="n">
-        <v>120.27</v>
+        <v>106.723333333333</v>
       </c>
       <c r="N8"/>
       <c r="O8" t="n">
-        <v>42.13</v>
+        <v>77.7666666666667</v>
       </c>
       <c r="P8"/>
       <c r="Q8" t="n">
-        <v>42.6</v>
+        <v>42.17</v>
       </c>
     </row>
     <row r="9">
@@ -9626,35 +9782,35 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="n">
-        <v>48.11</v>
+        <v>47.705</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="n">
-        <v>133.64</v>
+        <v>124.3</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>93.08</v>
+        <v>81.2433333333333</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="n">
-        <v>48.4</v>
+        <v>42.2633333333333</v>
       </c>
       <c r="J9"/>
       <c r="K9" t="n">
-        <v>83.75</v>
+        <v>76.0766666666667</v>
       </c>
       <c r="L9"/>
       <c r="M9" t="n">
-        <v>108.83</v>
+        <v>96.3883333333333</v>
       </c>
       <c r="N9"/>
       <c r="O9" t="n">
-        <v>43.38</v>
+        <v>83.375</v>
       </c>
       <c r="P9"/>
       <c r="Q9" t="n">
-        <v>46.2</v>
+        <v>45.7</v>
       </c>
     </row>
     <row r="10">
@@ -9663,35 +9819,35 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="n">
-        <v>34.89</v>
+        <v>35.5366666666667</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="n">
-        <v>98.88</v>
+        <v>93.5166666666667</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>92.13</v>
+        <v>85.555</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="n">
-        <v>23.38</v>
+        <v>24.5</v>
       </c>
       <c r="J10"/>
       <c r="K10" t="n">
-        <v>67.33</v>
+        <v>64.1566666666667</v>
       </c>
       <c r="L10"/>
       <c r="M10" t="n">
-        <v>115.77</v>
+        <v>100.751666666667</v>
       </c>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>27.24</v>
+        <v>57.0583333333333</v>
       </c>
       <c r="P10"/>
       <c r="Q10" t="n">
-        <v>62.47</v>
+        <v>61.0833333333333</v>
       </c>
     </row>
     <row r="11">
@@ -9700,35 +9856,35 @@
       </c>
       <c r="B11"/>
       <c r="C11" t="n">
-        <v>28.44</v>
+        <v>34.1666666666667</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="n">
-        <v>101.34</v>
+        <v>95.15</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>56.73</v>
+        <v>54.1566666666667</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="n">
-        <v>33.87</v>
+        <v>31.37</v>
       </c>
       <c r="J11"/>
       <c r="K11" t="n">
-        <v>56.4</v>
+        <v>54.7383333333333</v>
       </c>
       <c r="L11"/>
       <c r="M11" t="n">
-        <v>76.1</v>
+        <v>67.055</v>
       </c>
       <c r="N11"/>
       <c r="O11" t="n">
-        <v>36.8</v>
+        <v>67.6833333333333</v>
       </c>
       <c r="P11"/>
       <c r="Q11" t="n">
-        <v>30.67</v>
+        <v>30.1833333333333</v>
       </c>
     </row>
     <row r="12">
@@ -9737,35 +9893,35 @@
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>27.13</v>
+        <v>28.4233333333333</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="n">
-        <v>78.26</v>
+        <v>89.15</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>55.07</v>
+        <v>52.0666666666667</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="n">
-        <v>29.11</v>
+        <v>28.1333333333333</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="n">
-        <v>49.18</v>
+        <v>50.7333333333333</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="n">
-        <v>60.03</v>
+        <v>56.165</v>
       </c>
       <c r="N12"/>
       <c r="O12" t="n">
-        <v>20.09</v>
+        <v>36.4416666666667</v>
       </c>
       <c r="P12"/>
       <c r="Q12" t="n">
-        <v>21.47</v>
+        <v>21.0066666666667</v>
       </c>
     </row>
     <row r="13">
@@ -9774,35 +9930,35 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="n">
-        <v>28.4</v>
+        <v>27.1666666666667</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="n">
-        <v>84.38</v>
+        <v>76.5333333333333</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>40.12</v>
+        <v>37.2683333333333</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="n">
-        <v>28.18</v>
+        <v>24.72</v>
       </c>
       <c r="J13"/>
       <c r="K13" t="n">
-        <v>45.46</v>
+        <v>41.6583333333333</v>
       </c>
       <c r="L13"/>
       <c r="M13" t="n">
-        <v>61</v>
+        <v>53.2783333333333</v>
       </c>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>14.76</v>
+        <v>27.8416666666667</v>
       </c>
       <c r="P13"/>
       <c r="Q13" t="n">
-        <v>21.33</v>
+        <v>20.77</v>
       </c>
     </row>
     <row r="14">
@@ -9811,35 +9967,35 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="n">
-        <v>14.44</v>
+        <v>14.1666666666667</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="n">
-        <v>41.7</v>
+        <v>42.9833333333333</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>28.49</v>
+        <v>26.2883333333333</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="n">
-        <v>11.84</v>
+        <v>10.3883333333333</v>
       </c>
       <c r="J14"/>
       <c r="K14" t="n">
-        <v>25.14</v>
+        <v>24.3066666666667</v>
       </c>
       <c r="L14"/>
       <c r="M14" t="n">
-        <v>31.27</v>
+        <v>29.0816666666667</v>
       </c>
       <c r="N14"/>
       <c r="O14" t="n">
-        <v>10.04</v>
+        <v>17.9833333333333</v>
       </c>
       <c r="P14"/>
       <c r="Q14" t="n">
-        <v>7.73</v>
+        <v>7.65666666666667</v>
       </c>
     </row>
     <row r="15">
@@ -9848,33 +10004,33 @@
       </c>
       <c r="B15"/>
       <c r="C15" t="n">
-        <v>9.67</v>
+        <v>10.39</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="n">
-        <v>40.32</v>
+        <v>42.5333333333333</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>17.84</v>
+        <v>15.99</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="n">
-        <v>6.16</v>
+        <v>5.55666666666667</v>
       </c>
       <c r="J15"/>
       <c r="K15" t="n">
-        <v>18.91</v>
+        <v>18.8066666666667</v>
       </c>
       <c r="L15"/>
       <c r="M15" t="n">
-        <v>14</v>
+        <v>14.0025</v>
       </c>
       <c r="N15"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15" t="n">
-        <v>3.93</v>
+        <v>3.95333333333333</v>
       </c>
     </row>
     <row r="16">
@@ -9883,23 +10039,23 @@
       </c>
       <c r="B16"/>
       <c r="C16" t="n">
-        <v>4.15</v>
+        <v>4.6125</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="n">
-        <v>53.87</v>
+        <v>45.45</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>17.22</v>
+        <v>13.2625</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="n">
-        <v>4</v>
+        <v>3.1375</v>
       </c>
       <c r="J16"/>
       <c r="K16" t="n">
-        <v>20.24</v>
+        <v>16.82</v>
       </c>
       <c r="L16"/>
       <c r="M16"/>
@@ -9907,7 +10063,7 @@
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16" t="n">
-        <v>4.8</v>
+        <v>5.02</v>
       </c>
     </row>
   </sheetData>
@@ -9929,40 +10085,52 @@
         <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="F1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="H1" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="I1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="J1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="K1" t="s">
-        <v>236</v>
+        <v>292</v>
       </c>
       <c r="L1" t="s">
+        <v>293</v>
+      </c>
+      <c r="M1" t="s">
+        <v>294</v>
+      </c>
+      <c r="N1" t="s">
         <v>237</v>
       </c>
-      <c r="M1" t="s">
-        <v>288</v>
+      <c r="O1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P1" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="2">
@@ -9979,19 +10147,19 @@
         <v>236</v>
       </c>
       <c r="E2" t="n">
+        <v>236</v>
+      </c>
+      <c r="F2" t="n">
         <v>12</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>8</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>20</v>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -10003,6 +10171,18 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10020,19 +10200,19 @@
         <v>258</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>258</v>
       </c>
       <c r="F3" t="n">
         <v>10</v>
       </c>
       <c r="G3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" t="n">
         <v>20</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -10044,6 +10224,18 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10061,19 +10253,19 @@
         <v>494</v>
       </c>
       <c r="E4" t="n">
+        <v>494</v>
+      </c>
+      <c r="F4" t="n">
         <v>15</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>16</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>31</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -10085,6 +10277,18 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10102,19 +10306,19 @@
         <v>123</v>
       </c>
       <c r="E5" t="n">
+        <v>123</v>
+      </c>
+      <c r="F5" t="n">
         <v>7</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>8</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>15</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -10126,6 +10330,18 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10143,19 +10359,19 @@
         <v>1111</v>
       </c>
       <c r="E6" t="n">
+        <v>1111</v>
+      </c>
+      <c r="F6" t="n">
         <v>44</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>42</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>86</v>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -10167,6 +10383,18 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10184,19 +10412,19 @@
         <v>306</v>
       </c>
       <c r="E7" t="n">
+        <v>306</v>
+      </c>
+      <c r="F7" t="n">
         <v>4</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>9</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>13</v>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -10208,6 +10436,18 @@
         <v>0</v>
       </c>
       <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10225,30 +10465,42 @@
         <v>581</v>
       </c>
       <c r="E8" t="n">
+        <v>581</v>
+      </c>
+      <c r="F8" t="n">
         <v>6</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>19</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>25</v>
       </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
         <v>17.9</v>
       </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.50890782339272</v>
+      </c>
+      <c r="Q8" t="n">
         <v>17.9</v>
       </c>
     </row>
@@ -10266,28 +10518,40 @@
         <v>225</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>5</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
-      <c r="K9"/>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9"/>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10307,55 +10571,55 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="C1" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="E1" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="F1" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="G1" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="H1" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="I1" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="J1" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="K1" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="L1" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="M1" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="N1" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="O1" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="P1" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="Q1" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2">
@@ -10529,7 +10793,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2</v>
+        <v>0.0488348439977265</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -10541,7 +10805,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1</v>
+        <v>0.0320699708454811</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -10582,7 +10846,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5</v>
+        <v>0.130880873953922</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -10594,19 +10858,19 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3</v>
+        <v>0.0802105301104923</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.3</v>
+        <v>0.0969717693073702</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>1.4</v>
+        <v>0.495632672332389</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
@@ -10623,49 +10887,49 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3</v>
+        <v>0.078904391664004</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2</v>
+        <v>0.124058196934269</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1.2</v>
+        <v>0.680068827845762</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>1.2</v>
+        <v>0.32775418035304</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9</v>
+        <v>0.415157981868473</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2</v>
+        <v>0.18987788522623</v>
       </c>
       <c r="N7" t="n">
-        <v>1.7</v>
+        <v>1.50890782339272</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>0.628698800568405</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.4</v>
+        <v>4.56674683507056</v>
       </c>
     </row>
     <row r="8">
@@ -10674,35 +10938,35 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="n">
-        <v>1.9</v>
+        <v>0.608873342937638</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="n">
-        <v>1.4</v>
+        <v>0.441980002816505</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>1.6</v>
+        <v>0.872190368120737</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="n">
-        <v>2.2</v>
+        <v>1.32372550576218</v>
       </c>
       <c r="J8"/>
       <c r="K8" t="n">
-        <v>1.6</v>
+        <v>0.778380046701033</v>
       </c>
       <c r="L8"/>
       <c r="M8" t="n">
-        <v>1.1</v>
+        <v>1.43071258556743</v>
       </c>
       <c r="N8"/>
       <c r="O8" t="n">
-        <v>1.1</v>
+        <v>0.782545563530573</v>
       </c>
       <c r="P8"/>
       <c r="Q8" t="n">
-        <v>5.1</v>
+        <v>4.44464285714286</v>
       </c>
     </row>
     <row r="9">
@@ -10711,35 +10975,35 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="n">
-        <v>1.2</v>
+        <v>0.892646610088262</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="n">
-        <v>1.4</v>
+        <v>1.07996078299518</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>2.2</v>
+        <v>2.11773385898108</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="n">
-        <v>3.3</v>
+        <v>1.795590295031</v>
       </c>
       <c r="J9"/>
       <c r="K9" t="n">
-        <v>1.9</v>
+        <v>1.52313889704446</v>
       </c>
       <c r="L9"/>
       <c r="M9" t="n">
-        <v>4.7</v>
+        <v>4.86415334995998</v>
       </c>
       <c r="N9"/>
       <c r="O9" t="n">
-        <v>2.1</v>
+        <v>2.18499439190477</v>
       </c>
       <c r="P9"/>
       <c r="Q9" t="n">
-        <v>1.4</v>
+        <v>1.13333333333333</v>
       </c>
     </row>
     <row r="10">
@@ -10748,35 +11012,35 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>3.87768465648582</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="n">
-        <v>0.9</v>
+        <v>0.999097435857026</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>4.8</v>
+        <v>4.397787656191</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="n">
-        <v>5.4</v>
+        <v>4.64047188482294</v>
       </c>
       <c r="J10"/>
       <c r="K10" t="n">
-        <v>3.5</v>
+        <v>3.344914048253</v>
       </c>
       <c r="L10"/>
       <c r="M10" t="n">
-        <v>2.7</v>
+        <v>1.98559838533558</v>
       </c>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>2.5</v>
+        <v>5.65622564076896</v>
       </c>
       <c r="P10"/>
       <c r="Q10" t="n">
-        <v>1.1</v>
+        <v>1.43319268635724</v>
       </c>
     </row>
     <row r="11">
@@ -10785,35 +11049,35 @@
       </c>
       <c r="B11"/>
       <c r="C11" t="n">
-        <v>6.3</v>
+        <v>7.34184112640905</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="n">
-        <v>2.2</v>
+        <v>2.83790535304474</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>4.3</v>
+        <v>5.20568565768097</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="n">
-        <v>7</v>
+        <v>9.03245343614529</v>
       </c>
       <c r="J11"/>
       <c r="K11" t="n">
-        <v>4.1</v>
+        <v>4.87597843391547</v>
       </c>
       <c r="L11"/>
       <c r="M11" t="n">
-        <v>4.8</v>
+        <v>6.59683973903415</v>
       </c>
       <c r="N11"/>
       <c r="O11" t="n">
-        <v>7.6</v>
+        <v>6.08469567678925</v>
       </c>
       <c r="P11"/>
       <c r="Q11" t="n">
-        <v>4.6</v>
+        <v>4.06675527987003</v>
       </c>
     </row>
     <row r="12">
@@ -10822,35 +11086,35 @@
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>5.8</v>
+        <v>5.24863510057424</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="n">
-        <v>5.6</v>
+        <v>8.30504157843965</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>4.6</v>
+        <v>5.873634499645</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="n">
-        <v>7.9</v>
+        <v>9.11117884098841</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="n">
-        <v>5.5</v>
+        <v>7.38337341125182</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="n">
-        <v>6.2</v>
+        <v>6.4259319972273</v>
       </c>
       <c r="N12"/>
       <c r="O12" t="n">
-        <v>1.1</v>
+        <v>3.41666666666667</v>
       </c>
       <c r="P12"/>
       <c r="Q12" t="n">
-        <v>3.1</v>
+        <v>1.8000773395205</v>
       </c>
     </row>
     <row r="13">
@@ -10859,35 +11123,35 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="n">
-        <v>6.2</v>
+        <v>6.74058657885458</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="n">
-        <v>4.1</v>
+        <v>6.0322123246442</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>8.2</v>
+        <v>7.78087306946193</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="n">
-        <v>10.3</v>
+        <v>7.90710682396344</v>
       </c>
       <c r="J13"/>
       <c r="K13" t="n">
-        <v>6.5</v>
+        <v>7.0972450593708</v>
       </c>
       <c r="L13"/>
       <c r="M13" t="n">
-        <v>4</v>
+        <v>3.3564097551144</v>
       </c>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>6.6</v>
+        <v>5.74742256125751</v>
       </c>
       <c r="P13"/>
       <c r="Q13" t="n">
-        <v>3.2</v>
+        <v>1.59990047275442</v>
       </c>
     </row>
     <row r="14">
@@ -10896,31 +11160,31 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="n">
-        <v>6.7</v>
+        <v>6.02728231102489</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="n">
-        <v>6.7</v>
+        <v>7.28962859503049</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>10.6</v>
+        <v>16.2936251843193</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="n">
-        <v>10</v>
+        <v>12.0987110058103</v>
       </c>
       <c r="J14"/>
       <c r="K14" t="n">
-        <v>8.6</v>
+        <v>10.1003936779959</v>
       </c>
       <c r="L14"/>
       <c r="M14" t="n">
-        <v>9.6</v>
+        <v>9.40586588639755</v>
       </c>
       <c r="N14"/>
       <c r="O14" t="n">
-        <v>6.8</v>
+        <v>4.32644059763915</v>
       </c>
       <c r="P14"/>
       <c r="Q14" t="n">
@@ -10933,27 +11197,27 @@
       </c>
       <c r="B15"/>
       <c r="C15" t="n">
-        <v>5.6</v>
+        <v>6.21877765730218</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="n">
-        <v>2.1</v>
+        <v>1.70444150216659</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>4.7</v>
+        <v>3.10651777155021</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="n">
-        <v>5.1</v>
+        <v>10.4948443449717</v>
       </c>
       <c r="J15"/>
       <c r="K15" t="n">
-        <v>3.7</v>
+        <v>3.27578456958708</v>
       </c>
       <c r="L15"/>
       <c r="M15" t="n">
-        <v>9.4</v>
+        <v>37.3883821648646</v>
       </c>
       <c r="N15"/>
       <c r="O15"/>
@@ -10968,15 +11232,15 @@
       </c>
       <c r="B16"/>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2.27916666666667</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="n">
-        <v>3.5</v>
+        <v>3.84654422306516</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>2.2</v>
+        <v>3.41720491754739</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="n">
@@ -10984,7 +11248,7 @@
       </c>
       <c r="J16"/>
       <c r="K16" t="n">
-        <v>2.7</v>
+        <v>4.08348539424126</v>
       </c>
       <c r="L16"/>
       <c r="M16"/>

</xml_diff>